<commit_message>
Removed the met file path in Apsim file
</commit_message>
<xml_diff>
--- a/Tests/Validation/Ryegrass/Observed.xlsx
+++ b/Tests/Validation/Ryegrass/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jessica\GIT\ApsimX\ApsimX\Tests\Validation\Ryegrass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C70295A-6A78-4768-A526-EAB15FB9447F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2F8E39-9AB3-46F6-AD22-E105EEA954E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43080" yWindow="-3975" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>AgPRyegrass.Leaf.Dead.Wt</t>
   </si>
   <si>
-    <t>AgPRyegrass.AboveGround.NConc</t>
-  </si>
-  <si>
     <t>AgPRyegrass.Leaf.Live.NConc</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>AgPRyegrass.Harvestable.Digestibility</t>
+  </si>
+  <si>
+    <t>AgPRyegrass.AboveGroundNConc</t>
   </si>
 </sst>
 </file>
@@ -398,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -432,13 +432,13 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -450,13 +450,13 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">

</xml_diff>